<commit_message>
21-4140 post-go-live: new submission
</commit_message>
<xml_diff>
--- a/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
+++ b/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t xml:space="preserve">21-4140 Post-Go-Live Submission Tracker</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">f21ac25a-5b26-41ce-a64d-eb1eb7d44a21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">processing</t>
   </si>
 </sst>
 </file>
@@ -471,7 +468,7 @@
   <dimension ref="A1:F376"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -755,10 +752,14 @@
         <v>46061.4597222222</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>46060.4180555556</v>
+      </c>
+      <c r="F21" s="7" t="n">
+        <v>68769153</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6"/>

</xml_diff>

<commit_message>
21-4140 update total expected submissions
</commit_message>
<xml_diff>
--- a/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
+++ b/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t xml:space="preserve">21-4140 Post-Go-Live Submission Tracker</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">f21ac25a-5b26-41ce-a64d-eb1eb7d44a21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
   </sheetPr>
   <dimension ref="A1:F376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -491,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>3000</v>
+        <v>3807</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -503,11 +506,11 @@
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">COUNTIF(A11:A70,"*")-COUNT(A11:A70)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">B4/B3</f>
-        <v>0.00366666666666667</v>
+        <v>0.00341476228001051</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,24 +758,32 @@
         <v>13</v>
       </c>
       <c r="E21" s="10" t="n">
-        <v>46060.4180555556</v>
+        <v>46061.4180555556</v>
       </c>
       <c r="F21" s="7" t="n">
         <v>68769153</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
+      <c r="A22" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="10" t="n">
+        <v>46062.4354166667</v>
+      </c>
       <c r="D22" s="7"/>
       <c r="E22" s="10"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
+      <c r="A23" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="10"/>
+      <c r="C23" s="10" t="n">
+        <v>46062.8694444444</v>
+      </c>
       <c r="D23" s="7"/>
       <c r="E23" s="10"/>
       <c r="F23" s="9"/>

</xml_diff>

<commit_message>
21-4140 post go live tracker updates
</commit_message>
<xml_diff>
--- a/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
+++ b/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t xml:space="preserve">21-4140 Post-Go-Live Submission Tracker</t>
   </si>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">b8a5ae78-2939-4ad6-90e4-14cdbd621398</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">c80b6b8a-e5c8-482b-8f88-633dd41441c6</t>
   </si>
   <si>
@@ -97,7 +94,31 @@
     <t xml:space="preserve">f21ac25a-5b26-41ce-a64d-eb1eb7d44a21</t>
   </si>
   <si>
-    <t xml:space="preserve">.</t>
+    <t xml:space="preserve">c7010f85-2a8b-47e2-bd99-3a45bff61b4e</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vbms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fa5b0a1f-2ca3-4ed2-9e8f-21d29b188ad8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">056cc35c-d270-4f62-b696-65fced00fd51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87efed84-a179-49ec-9d0d-c4d29c9b2a1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b8c73c9c-1edb-4a7a-aff1-c20ea37e5816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3e874961-c725-40be-861f-09b1fc3511d6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26c58d71-8daf-460d-b6eb-59b4f4974912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">224f98e7-98b6-41ed-9366-5f39d1a3409f</t>
   </si>
 </sst>
 </file>
@@ -110,7 +131,7 @@
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -157,6 +178,12 @@
     <font>
       <sz val="10"/>
       <name val="Cascadia Code SemiBold"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Cascadia Mono SemiBold"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
@@ -226,7 +253,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,6 +304,10 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -471,7 +502,7 @@
   <dimension ref="A1:F376"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -506,11 +537,11 @@
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">COUNTIF(A11:A70,"*")-COUNT(A11:A70)</f>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">B4/B3</f>
-        <v>0.00341476228001051</v>
+        <v>0.00499080640924613</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,8 +602,8 @@
       <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>15</v>
+      <c r="C12" s="10" t="n">
+        <v>46058.4680555556</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>13</v>
@@ -586,7 +617,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>12</v>
@@ -606,7 +637,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>12</v>
@@ -626,7 +657,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>12</v>
@@ -646,7 +677,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>12</v>
@@ -666,7 +697,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>12</v>
@@ -686,7 +717,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>12</v>
@@ -706,7 +737,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>12</v>
@@ -726,7 +757,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>12</v>
@@ -746,7 +777,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>12</v>
@@ -765,10 +796,12 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="7"/>
       <c r="C22" s="10" t="n">
         <v>46062.4354166667</v>
       </c>
@@ -778,9 +811,11 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="7"/>
       <c r="C23" s="10" t="n">
         <v>46062.8694444444</v>
       </c>
@@ -789,49 +824,85 @@
       <c r="F23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="10" t="n">
+        <v>46064.7840277778</v>
+      </c>
       <c r="D24" s="7"/>
       <c r="E24" s="10"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="10" t="n">
+        <v>46065.4166666667</v>
+      </c>
       <c r="D25" s="7"/>
       <c r="E25" s="10"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="10" t="n">
+        <v>46065.5527777778</v>
+      </c>
       <c r="D26" s="7"/>
       <c r="E26" s="10"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="10"/>
+      <c r="A27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="10" t="n">
+        <v>46065.725</v>
+      </c>
       <c r="D27" s="7"/>
       <c r="E27" s="10"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="10" t="n">
+        <v>46034.8090277778</v>
+      </c>
       <c r="D28" s="7"/>
       <c r="E28" s="10"/>
       <c r="F28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="10"/>
+      <c r="A29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="10" t="n">
+        <v>46066.3798611111</v>
+      </c>
       <c r="D29" s="7"/>
       <c r="E29" s="10"/>
       <c r="F29" s="9"/>
@@ -1141,7 +1212,7 @@
       <c r="F67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="13"/>
+      <c r="A68" s="14"/>
       <c r="B68" s="7"/>
       <c r="C68" s="10"/>
       <c r="D68" s="7"/>
@@ -1149,7 +1220,7 @@
       <c r="F68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="13"/>
+      <c r="A69" s="14"/>
       <c r="B69" s="7"/>
       <c r="C69" s="10"/>
       <c r="D69" s="7"/>
@@ -1157,7 +1228,7 @@
       <c r="F69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="13"/>
+      <c r="A70" s="14"/>
       <c r="B70" s="7"/>
       <c r="C70" s="10"/>
       <c r="D70" s="7"/>

</xml_diff>

<commit_message>
21-4140 post-go-live updates excel file
</commit_message>
<xml_diff>
--- a/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
+++ b/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="56">
   <si>
     <t xml:space="preserve">21-4140 Post-Go-Live Submission Tracker</t>
   </si>
@@ -173,6 +173,21 @@
   </si>
   <si>
     <t xml:space="preserve">173cb54f-b5d1-4477-9a08-839017fd9798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54c3c280-f486-4bb3-9b95-c7de8e623521</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8be933b0-0354-48d7-94d5-f2abfd7e6b3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7d96ff2f-1070-4eee-99f0-7305245fb358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4901c4ad-8d73-4189-889a-b634fbfab1a8</t>
   </si>
 </sst>
 </file>
@@ -570,8 +585,8 @@
   </sheetPr>
   <dimension ref="A1:G376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A39:A43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -606,11 +621,11 @@
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">COUNTIF(A11:A70,"*")-COUNT(A11:A70)</f>
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5" t="n">
         <f aca="false">B4/B3</f>
-        <v>0.0086682427107959</v>
+        <v>0.00971893879695298</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,11 +633,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6" t="n">
         <f aca="false">B5/B3</f>
-        <v>0.00026267402153927</v>
+        <v>0.00131337010769635</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1224,9 +1239,15 @@
       <c r="C39" s="12" t="n">
         <v>46073.9548611111</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="11"/>
+      <c r="D39" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="12" t="n">
+        <v>46074.4486111111</v>
+      </c>
+      <c r="F39" s="11" t="n">
+        <v>69212086</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
@@ -1238,10 +1259,16 @@
       <c r="C40" s="12" t="n">
         <v>46074.1916666667</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="0" t="s">
+      <c r="D40" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="12" t="n">
+        <v>46074.15</v>
+      </c>
+      <c r="F40" s="11" t="n">
+        <v>69212650</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1255,10 +1282,16 @@
       <c r="C41" s="12" t="n">
         <v>46074.2298611111</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="0" t="s">
+      <c r="D41" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="12" t="n">
+        <v>46074.4701388889</v>
+      </c>
+      <c r="F41" s="11" t="n">
+        <v>69212684</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1272,9 +1305,15 @@
       <c r="C42" s="12" t="n">
         <v>46074.6340277778</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="11"/>
+      <c r="D42" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="12" t="n">
+        <v>46076.3597222222</v>
+      </c>
+      <c r="F42" s="11" t="n">
+        <v>69221624</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
@@ -1286,41 +1325,101 @@
       <c r="C43" s="12" t="n">
         <v>46075.8479166667</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="11"/>
+      <c r="D43" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="12" t="n">
+        <v>46076.4319444444</v>
+      </c>
+      <c r="F43" s="11" t="n">
+        <v>69228956</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="11"/>
+      <c r="A44" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="12" t="n">
+        <v>46077.4180555556</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="11"/>
+      <c r="A45" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="12" t="n">
+        <v>46077.5076388889</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="11"/>
+      <c r="A46" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="12" t="n">
+        <v>46077.7826388889</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="11"/>
+      <c r="A47" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="12" t="n">
+        <v>46078.0972222222</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="8"/>

</xml_diff>

<commit_message>
21-4140 post-go-live detials added to tracker
</commit_message>
<xml_diff>
--- a/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
+++ b/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
   <si>
     <t xml:space="preserve">21-4140 Post-Go-Live Submission Tracker</t>
   </si>
@@ -178,13 +178,13 @@
     <t xml:space="preserve">54c3c280-f486-4bb3-9b95-c7de8e623521</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">8be933b0-0354-48d7-94d5-f2abfd7e6b3d</t>
   </si>
   <si>
     <t xml:space="preserve">7d96ff2f-1070-4eee-99f0-7305245fb358</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Complete</t>
   </si>
   <si>
     <t xml:space="preserve">4901c4ad-8d73-4189-889a-b634fbfab1a8</t>
@@ -585,8 +585,8 @@
   </sheetPr>
   <dimension ref="A1:G376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1346,21 +1346,21 @@
         <v>46077.4180555556</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="12" t="n">
+        <v>46077.5305555556</v>
+      </c>
+      <c r="F44" s="11" t="n">
+        <v>69285905</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>26</v>
@@ -1369,21 +1369,21 @@
         <v>46077.5076388889</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G45" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="12" t="n">
+        <v>46077.6465277778</v>
+      </c>
+      <c r="F45" s="11" t="n">
+        <v>69294694</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>26</v>
@@ -1392,13 +1392,13 @@
         <v>46077.7826388889</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="E46" s="12" t="n">
+        <v>46077.9388888889</v>
+      </c>
+      <c r="F46" s="11" t="n">
+        <v>69324354</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1412,13 +1412,13 @@
         <v>46078.0972222222</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="E47" s="12" t="n">
+        <v>46078.4534722222</v>
+      </c>
+      <c r="F47" s="11" t="n">
+        <v>69331094</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
21-4140 post-go-live new submission for tracker and updated stats
</commit_message>
<xml_diff>
--- a/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
+++ b/teams/benefits-portfolio/benefits-intake-optimization-pingwind/post-go-live/21-4140/21-4140-post-go-live-submission-tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="59">
   <si>
     <t xml:space="preserve">21-4140 Post-Go-Live Submission Tracker</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t xml:space="preserve">4901c4ad-8d73-4189-889a-b634fbfab1a8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77e6a163-507a-40b6-8fb3-c13cc861f9c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31033a9b-fbe5-41ab-bdf3-4ce3cde56d6a</t>
   </si>
 </sst>
 </file>
@@ -585,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:G376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -621,11 +630,11 @@
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">COUNTIF(A11:A70,"*")-COUNT(A11:A70)</f>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C4" s="5" t="n">
         <f aca="false">B4/B3</f>
-        <v>0.00971893879695298</v>
+        <v>0.0102442868400315</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,19 +1431,39 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="12"/>
+      <c r="A48" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="12" t="n">
+        <v>46078.8111111111</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="F48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="12"/>
+      <c r="A49" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="12" t="n">
+        <v>46078.9131944444</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="F49" s="11"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>